<commit_message>
Conditional step head model workds from [-7, 7, 1] in 3 steps. Now need to refactor TrajectorySampler. No need to zero advantages after peaks.
</commit_message>
<xml_diff>
--- a/experiments/pg/start_from_m7_7_m7_max_step_7_step_num_3_cond_step_head_return_mode_max/oracle_buffer.xlsx
+++ b/experiments/pg/start_from_m7_7_m7_max_step_7_step_num_3_cond_step_head_return_mode_max/oracle_buffer.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C296"/>
+  <dimension ref="A1:C295"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1348,11 +1348,11 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>[-7, 2, -1]</t>
+          <t>[-2, 3, -7]</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>-0.004490505448061402</v>
+        <v>-0.004536752257632073</v>
       </c>
     </row>
     <row r="72">
@@ -1361,11 +1361,11 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>[-2, 3, -7]</t>
+          <t>[-2, -3, -7]</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>-0.004536752257632073</v>
+        <v>-0.004434604412261497</v>
       </c>
     </row>
     <row r="73">
@@ -1374,11 +1374,11 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>[-2, -3, -7]</t>
+          <t>[-4, 6, -7]</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>-0.004434604412261497</v>
+        <v>-0.004743845279956893</v>
       </c>
     </row>
     <row r="74">
@@ -1387,11 +1387,11 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>[-4, 6, -7]</t>
+          <t>[-6, 2, -7]</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>-0.004743845279956893</v>
+        <v>-0.004467518826875296</v>
       </c>
     </row>
     <row r="75">
@@ -1400,11 +1400,11 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>[-6, 2, -7]</t>
+          <t>[-6, 2, -3]</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>-0.004467518826875296</v>
+        <v>-0.004447847927903625</v>
       </c>
     </row>
     <row r="76">
@@ -1413,11 +1413,11 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>[-6, 2, -3]</t>
+          <t>[-7, -2, -7]</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>-0.004447847927903625</v>
+        <v>-0.004471277736310095</v>
       </c>
     </row>
     <row r="77">
@@ -1426,11 +1426,11 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>[-7, -2, -7]</t>
+          <t>[1, 7, -7]</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>-0.004471277736310095</v>
+        <v>-0.004745034349642029</v>
       </c>
     </row>
     <row r="78">
@@ -1439,11 +1439,11 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>[1, 7, -7]</t>
+          <t>[-4, 1, -7]</t>
         </is>
       </c>
       <c r="C78" t="n">
-        <v>-0.004745034349642029</v>
+        <v>-0.003759426728144985</v>
       </c>
     </row>
     <row r="79">
@@ -1452,11 +1452,11 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>[-4, 1, -7]</t>
+          <t>[-3, 4, -7]</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>-0.003759426728144985</v>
+        <v>-0.00466940171914932</v>
       </c>
     </row>
     <row r="80">
@@ -1465,11 +1465,11 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>[-3, 4, -7]</t>
+          <t>[-7, 3, -6]</t>
         </is>
       </c>
       <c r="C80" t="n">
-        <v>-0.00466940171914932</v>
+        <v>-0.004631963222782069</v>
       </c>
     </row>
     <row r="81">
@@ -1478,11 +1478,11 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>[-7, 3, -6]</t>
+          <t>[-7, 5, -6]</t>
         </is>
       </c>
       <c r="C81" t="n">
-        <v>-0.004631963222782069</v>
+        <v>-0.00473047147008163</v>
       </c>
     </row>
     <row r="82">
@@ -1491,11 +1491,11 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>[-7, 5, -6]</t>
+          <t>[-7, 7, 1]</t>
         </is>
       </c>
       <c r="C82" t="n">
-        <v>-0.00473047147008163</v>
+        <v>-0.00474345512998797</v>
       </c>
     </row>
     <row r="83">
@@ -1504,11 +1504,11 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>[-7, 7, 1]</t>
+          <t>[-7, -7, -7]</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>-0.00474345512998797</v>
+        <v>-0.004745940003927722</v>
       </c>
     </row>
     <row r="84">
@@ -1517,11 +1517,11 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>[-7, -7, -7]</t>
+          <t>[-5, 2, -3]</t>
         </is>
       </c>
       <c r="C84" t="n">
-        <v>-0.004745940003927722</v>
+        <v>-0.004389819311439473</v>
       </c>
     </row>
     <row r="85">
@@ -1530,11 +1530,11 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>[-5, 2, -3]</t>
+          <t>[-7, -4, -7]</t>
         </is>
       </c>
       <c r="C85" t="n">
-        <v>-0.004389819311439473</v>
+        <v>-0.004674622295602608</v>
       </c>
     </row>
     <row r="86">
@@ -1543,11 +1543,11 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>[-7, -4, -7]</t>
+          <t>[0, 0, -7]</t>
         </is>
       </c>
       <c r="C86" t="n">
-        <v>-0.004674622295602608</v>
+        <v>0.0007614180299048523</v>
       </c>
     </row>
     <row r="87">
@@ -1556,11 +1556,11 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>[0, 0, -7]</t>
+          <t>[0, 4, -7]</t>
         </is>
       </c>
       <c r="C87" t="n">
-        <v>0.0007614180299048523</v>
+        <v>-0.004665084832249327</v>
       </c>
     </row>
     <row r="88">
@@ -1569,11 +1569,11 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>[0, 4, -7]</t>
+          <t>[-7, 5, -4]</t>
         </is>
       </c>
       <c r="C88" t="n">
-        <v>-0.004665084832249327</v>
+        <v>-0.004728774492807817</v>
       </c>
     </row>
     <row r="89">
@@ -1582,11 +1582,11 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>[-7, 5, -4]</t>
+          <t>[-1, 6, -7]</t>
         </is>
       </c>
       <c r="C89" t="n">
-        <v>-0.004728774492807817</v>
+        <v>-0.004743674873253409</v>
       </c>
     </row>
     <row r="90">
@@ -1595,11 +1595,11 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>[-1, 6, -7]</t>
+          <t>[-3, 3, -7]</t>
         </is>
       </c>
       <c r="C90" t="n">
-        <v>-0.004743674873253409</v>
+        <v>-0.004547862050311155</v>
       </c>
     </row>
     <row r="91">
@@ -1608,11 +1608,11 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>[-3, 3, -7]</t>
+          <t>[-7, 0, -3]</t>
         </is>
       </c>
       <c r="C91" t="n">
-        <v>-0.004547862050311155</v>
+        <v>-0.004190478404269218</v>
       </c>
     </row>
     <row r="92">
@@ -1621,11 +1621,11 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>[-7, 0, -3]</t>
+          <t>[-3, 0, -7]</t>
         </is>
       </c>
       <c r="C92" t="n">
-        <v>-0.004190478404269218</v>
+        <v>-0.001743051689956108</v>
       </c>
     </row>
     <row r="93">
@@ -1634,11 +1634,11 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>[-3, 0, -7]</t>
+          <t>[3, 0, -7]</t>
         </is>
       </c>
       <c r="C93" t="n">
-        <v>-0.001743051689956108</v>
+        <v>-0.003215135358083213</v>
       </c>
     </row>
     <row r="94">
@@ -1647,11 +1647,11 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>[3, 0, -7]</t>
+          <t>[-3, 7, -6]</t>
         </is>
       </c>
       <c r="C94" t="n">
-        <v>-0.003215135358083213</v>
+        <v>-0.00474447906766993</v>
       </c>
     </row>
     <row r="95">
@@ -1660,11 +1660,11 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>[-3, 7, -6]</t>
+          <t>[-7, 7, 7]</t>
         </is>
       </c>
       <c r="C95" t="n">
-        <v>-0.00474447906766993</v>
+        <v>-0.00474493788946243</v>
       </c>
     </row>
     <row r="96">
@@ -1673,11 +1673,11 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>[-7, 7, 7]</t>
+          <t>[-7, 1, -6]</t>
         </is>
       </c>
       <c r="C96" t="n">
-        <v>-0.00474493788946243</v>
+        <v>-0.004379576511085032</v>
       </c>
     </row>
     <row r="97">
@@ -1686,11 +1686,11 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>[-7, 1, -6]</t>
+          <t>[-7, 5, -5]</t>
         </is>
       </c>
       <c r="C97" t="n">
-        <v>-0.004379576511085032</v>
+        <v>-0.004729642585015254</v>
       </c>
     </row>
     <row r="98">
@@ -1699,11 +1699,11 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>[-7, 5, -5]</t>
+          <t>[-7, -1, -5]</t>
         </is>
       </c>
       <c r="C98" t="n">
-        <v>-0.004729642585015254</v>
+        <v>-0.004292497108666559</v>
       </c>
     </row>
     <row r="99">
@@ -1712,11 +1712,11 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>[-7, -1, -5]</t>
+          <t>[-7, 6, 2]</t>
         </is>
       </c>
       <c r="C99" t="n">
-        <v>-0.004292497108666559</v>
+        <v>-0.00474251749419393</v>
       </c>
     </row>
     <row r="100">
@@ -1725,11 +1725,11 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>[-7, 6, 2]</t>
+          <t>[-7, 1, 0]</t>
         </is>
       </c>
       <c r="C100" t="n">
-        <v>-0.00474251749419393</v>
+        <v>-0.004307681063957049</v>
       </c>
     </row>
     <row r="101">
@@ -1738,11 +1738,11 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>[-7, 1, 0]</t>
+          <t>[-5, 0, -7]</t>
         </is>
       </c>
       <c r="C101" t="n">
-        <v>-0.004307681063957049</v>
+        <v>-0.003627007761583781</v>
       </c>
     </row>
     <row r="102">
@@ -1751,11 +1751,11 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>[-5, 0, -7]</t>
+          <t>[-6, 0, -7]</t>
         </is>
       </c>
       <c r="C102" t="n">
-        <v>-0.003627007761583781</v>
+        <v>-0.004046106816911508</v>
       </c>
     </row>
     <row r="103">
@@ -1764,11 +1764,11 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>[-6, 0, -7]</t>
+          <t>[-7, 7, 3]</t>
         </is>
       </c>
       <c r="C103" t="n">
-        <v>-0.004046106816911508</v>
+        <v>-0.004743668713282668</v>
       </c>
     </row>
     <row r="104">
@@ -1777,11 +1777,11 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>[-7, 7, 3]</t>
+          <t>[6, 2, -7]</t>
         </is>
       </c>
       <c r="C104" t="n">
-        <v>-0.004743668713282668</v>
+        <v>-0.004528204704483002</v>
       </c>
     </row>
     <row r="105">
@@ -1790,11 +1790,11 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>[6, 2, -7]</t>
+          <t>[-3, 7, -4]</t>
         </is>
       </c>
       <c r="C105" t="n">
-        <v>-0.004528204704483002</v>
+        <v>-0.004743622619139449</v>
       </c>
     </row>
     <row r="106">
@@ -1803,11 +1803,11 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>[-3, 7, -4]</t>
+          <t>[-7, 2, -2]</t>
         </is>
       </c>
       <c r="C106" t="n">
-        <v>-0.004743622619139449</v>
+        <v>-0.004493407639366303</v>
       </c>
     </row>
     <row r="107">
@@ -1816,11 +1816,11 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>[-7, 2, -2]</t>
+          <t>[-7, -2, -2]</t>
         </is>
       </c>
       <c r="C107" t="n">
-        <v>-0.004493407639366303</v>
+        <v>-0.004426454223955521</v>
       </c>
     </row>
     <row r="108">
@@ -1829,11 +1829,11 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>[-7, -2, -2]</t>
+          <t>[-7, -5, -7]</t>
         </is>
       </c>
       <c r="C108" t="n">
-        <v>-0.004426454223955521</v>
+        <v>-0.004718998794162766</v>
       </c>
     </row>
     <row r="109">
@@ -1842,11 +1842,11 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>[-7, -5, -7]</t>
+          <t>[3, 6, -7]</t>
         </is>
       </c>
       <c r="C109" t="n">
-        <v>-0.004718998794162766</v>
+        <v>-0.004744053700739709</v>
       </c>
     </row>
     <row r="110">
@@ -1855,11 +1855,11 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>[3, 6, -7]</t>
+          <t>[-4, 3, -7]</t>
         </is>
       </c>
       <c r="C110" t="n">
-        <v>-0.004744053700739709</v>
+        <v>-0.004564585577823672</v>
       </c>
     </row>
     <row r="111">
@@ -1868,11 +1868,11 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>[-4, 3, -7]</t>
+          <t>[0, 2, -7]</t>
         </is>
       </c>
       <c r="C111" t="n">
-        <v>-0.004564585577823672</v>
+        <v>-0.0041977070810701</v>
       </c>
     </row>
     <row r="112">
@@ -1881,11 +1881,11 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>[0, 2, -7]</t>
+          <t>[-1, 7, -5]</t>
         </is>
       </c>
       <c r="C112" t="n">
-        <v>-0.0041977070810701</v>
+        <v>-0.00474433324570989</v>
       </c>
     </row>
     <row r="113">
@@ -1894,11 +1894,11 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>[-1, 7, -5]</t>
+          <t>[0, 6, -7]</t>
         </is>
       </c>
       <c r="C113" t="n">
-        <v>-0.00474433324570989</v>
+        <v>-0.004743713211661364</v>
       </c>
     </row>
     <row r="114">
@@ -1907,11 +1907,11 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>[0, 6, -7]</t>
+          <t>[-1, 7, -1]</t>
         </is>
       </c>
       <c r="C114" t="n">
-        <v>-0.004743713211661364</v>
+        <v>-0.004742289822998163</v>
       </c>
     </row>
     <row r="115">
@@ -1920,11 +1920,11 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>[-1, 7, -1]</t>
+          <t>[-1, 1, -7]</t>
         </is>
       </c>
       <c r="C115" t="n">
-        <v>-0.004742289822998163</v>
+        <v>-0.003035540200074778</v>
       </c>
     </row>
     <row r="116">
@@ -1933,11 +1933,11 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>[-1, 1, -7]</t>
+          <t>[-1, 1, -1]</t>
         </is>
       </c>
       <c r="C116" t="n">
-        <v>-0.003035540200074778</v>
+        <v>-0.002871982403046364</v>
       </c>
     </row>
     <row r="117">
@@ -1946,11 +1946,11 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>[-1, 1, -1]</t>
+          <t>[-7, 0, -1]</t>
         </is>
       </c>
       <c r="C117" t="n">
-        <v>-0.002871982403046364</v>
+        <v>-0.004168315535900915</v>
       </c>
     </row>
     <row r="118">
@@ -1959,11 +1959,11 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>[-7, 0, -1]</t>
+          <t>[0, 3, -7]</t>
         </is>
       </c>
       <c r="C118" t="n">
-        <v>-0.004168315535900915</v>
+        <v>-0.004533071536011524</v>
       </c>
     </row>
     <row r="119">
@@ -1972,11 +1972,11 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>[0, 3, -7]</t>
+          <t>[-4, 3, 0]</t>
         </is>
       </c>
       <c r="C119" t="n">
-        <v>-0.004533071536011524</v>
+        <v>-0.004556948927938457</v>
       </c>
     </row>
     <row r="120">
@@ -1985,11 +1985,11 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>[-4, 3, 0]</t>
+          <t>[-3, 7, -1]</t>
         </is>
       </c>
       <c r="C120" t="n">
-        <v>-0.004556948927938457</v>
+        <v>-0.004741998433023747</v>
       </c>
     </row>
     <row r="121">
@@ -1998,11 +1998,11 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>[-3, 7, -1]</t>
+          <t>[-2, 7, -1]</t>
         </is>
       </c>
       <c r="C121" t="n">
-        <v>-0.004741998433023747</v>
+        <v>-0.004742025829341774</v>
       </c>
     </row>
     <row r="122">
@@ -2011,11 +2011,11 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>[-2, 7, -1]</t>
+          <t>[-4, 4, -7]</t>
         </is>
       </c>
       <c r="C122" t="n">
-        <v>-0.004742025829341774</v>
+        <v>-0.004674316839902757</v>
       </c>
     </row>
     <row r="123">
@@ -2024,11 +2024,11 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>[-4, 4, -7]</t>
+          <t>[0, 7, -3]</t>
         </is>
       </c>
       <c r="C123" t="n">
-        <v>-0.004674316839902757</v>
+        <v>-0.004743706285589558</v>
       </c>
     </row>
     <row r="124">
@@ -2037,11 +2037,11 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>[0, 7, -3]</t>
+          <t>[-3, 7, -3]</t>
         </is>
       </c>
       <c r="C124" t="n">
-        <v>-0.004743706285589558</v>
+        <v>-0.00474305822184184</v>
       </c>
     </row>
     <row r="125">
@@ -2050,11 +2050,11 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>[-3, 7, -3]</t>
+          <t>[-5, 6, -7]</t>
         </is>
       </c>
       <c r="C125" t="n">
-        <v>-0.00474305822184184</v>
+        <v>-0.004744039112442144</v>
       </c>
     </row>
     <row r="126">
@@ -2063,11 +2063,11 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>[-5, 6, -7]</t>
+          <t>[-6, 7, -5]</t>
         </is>
       </c>
       <c r="C126" t="n">
-        <v>-0.004744039112442144</v>
+        <v>-0.004744461641002915</v>
       </c>
     </row>
     <row r="127">
@@ -2076,11 +2076,11 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>[-6, 7, -5]</t>
+          <t>[-1, 4, -7]</t>
         </is>
       </c>
       <c r="C127" t="n">
-        <v>-0.004744461641002915</v>
+        <v>-0.004664796173173364</v>
       </c>
     </row>
     <row r="128">
@@ -2089,11 +2089,11 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>[-1, 4, -7]</t>
+          <t>[-2, 5, -7]</t>
         </is>
       </c>
       <c r="C128" t="n">
-        <v>-0.004664796173173364</v>
+        <v>-0.004722510359362992</v>
       </c>
     </row>
     <row r="129">
@@ -2102,11 +2102,11 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>[-2, 5, -7]</t>
+          <t>[-2, 1, -7]</t>
         </is>
       </c>
       <c r="C129" t="n">
-        <v>-0.004722510359362992</v>
+        <v>-0.003179709519689233</v>
       </c>
     </row>
     <row r="130">
@@ -2115,11 +2115,11 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>[-2, 1, -7]</t>
+          <t>[-1, 3, -7]</t>
         </is>
       </c>
       <c r="C130" t="n">
-        <v>-0.003179709519689233</v>
+        <v>-0.00453179114441871</v>
       </c>
     </row>
     <row r="131">
@@ -2128,11 +2128,11 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>[-1, 3, -7]</t>
+          <t>[-1, -4, -7]</t>
         </is>
       </c>
       <c r="C131" t="n">
-        <v>-0.00453179114441871</v>
+        <v>-0.004621850729256883</v>
       </c>
     </row>
     <row r="132">
@@ -2141,11 +2141,11 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>[-1, -4, -7]</t>
+          <t>[7, 7, -7]</t>
         </is>
       </c>
       <c r="C132" t="n">
-        <v>-0.004621850729256883</v>
+        <v>-0.004745884552805394</v>
       </c>
     </row>
     <row r="133">
@@ -2154,11 +2154,11 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>[7, 7, -7]</t>
+          <t>[-7, 1, -1]</t>
         </is>
       </c>
       <c r="C133" t="n">
-        <v>-0.004745884552805394</v>
+        <v>-0.004308607716742166</v>
       </c>
     </row>
     <row r="134">
@@ -2167,11 +2167,11 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>[-7, 1, -1]</t>
+          <t>[5, 7, -7]</t>
         </is>
       </c>
       <c r="C134" t="n">
-        <v>-0.004308607716742166</v>
+        <v>-0.004745509906650403</v>
       </c>
     </row>
     <row r="135">
@@ -2180,11 +2180,11 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>[5, 7, -7]</t>
+          <t>[4, 7, -7]</t>
         </is>
       </c>
       <c r="C135" t="n">
-        <v>-0.004745509906650403</v>
+        <v>-0.00474536445470079</v>
       </c>
     </row>
     <row r="136">
@@ -2193,11 +2193,11 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>[4, 7, -7]</t>
+          <t>[-7, -6, -7]</t>
         </is>
       </c>
       <c r="C136" t="n">
-        <v>-0.00474536445470079</v>
+        <v>-0.004740095456321267</v>
       </c>
     </row>
     <row r="137">
@@ -2206,11 +2206,11 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>[-7, -6, -7]</t>
+          <t>[-6, -6, -7]</t>
         </is>
       </c>
       <c r="C137" t="n">
-        <v>-0.004740095456321267</v>
+        <v>-0.004738917228373873</v>
       </c>
     </row>
     <row r="138">
@@ -2219,11 +2219,11 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>[-6, -6, -7]</t>
+          <t>[-1, -5, -7]</t>
         </is>
       </c>
       <c r="C138" t="n">
-        <v>-0.004738917228373873</v>
+        <v>-0.004703128120869965</v>
       </c>
     </row>
     <row r="139">
@@ -2232,11 +2232,11 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>[-1, -5, -7]</t>
+          <t>[1, 7, -2]</t>
         </is>
       </c>
       <c r="C139" t="n">
-        <v>-0.004703128120869965</v>
+        <v>-0.0047436013784039</v>
       </c>
     </row>
     <row r="140">
@@ -2245,11 +2245,11 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>[1, 7, -2]</t>
+          <t>[-7, 6, -3]</t>
         </is>
       </c>
       <c r="C140" t="n">
-        <v>-0.0047436013784039</v>
+        <v>-0.004743064344777535</v>
       </c>
     </row>
     <row r="141">
@@ -2258,11 +2258,11 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>[-7, 6, -3]</t>
+          <t>[-7, 6, 3]</t>
         </is>
       </c>
       <c r="C141" t="n">
-        <v>-0.004743064344777535</v>
+        <v>-0.00474268528457594</v>
       </c>
     </row>
     <row r="142">
@@ -2271,11 +2271,11 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>[-7, 6, 3]</t>
+          <t>[-1, -7, -7]</t>
         </is>
       </c>
       <c r="C142" t="n">
-        <v>-0.00474268528457594</v>
+        <v>-0.004745634555023063</v>
       </c>
     </row>
     <row r="143">
@@ -2284,11 +2284,11 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>[-1, -7, -7]</t>
+          <t>[-7, 6, 0]</t>
         </is>
       </c>
       <c r="C143" t="n">
-        <v>-0.004745634555023063</v>
+        <v>-0.004742458510846661</v>
       </c>
     </row>
     <row r="144">
@@ -2297,11 +2297,11 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>[-7, 6, 0]</t>
+          <t>[-6, 4, -7]</t>
         </is>
       </c>
       <c r="C144" t="n">
-        <v>-0.004742458510846661</v>
+        <v>-0.00468890809632403</v>
       </c>
     </row>
     <row r="145">
@@ -2310,11 +2310,11 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>[-6, 4, -7]</t>
+          <t>[-6, 6, -7]</t>
         </is>
       </c>
       <c r="C145" t="n">
-        <v>-0.00468890809632403</v>
+        <v>-0.004744332556752958</v>
       </c>
     </row>
     <row r="146">
@@ -2323,11 +2323,11 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>[-6, 6, -7]</t>
+          <t>[-5, 6, -3]</t>
         </is>
       </c>
       <c r="C146" t="n">
-        <v>-0.004744332556752958</v>
+        <v>-0.00474229742353735</v>
       </c>
     </row>
     <row r="147">
@@ -2336,11 +2336,11 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>[-5, 6, -3]</t>
+          <t>[-2, 6, -7]</t>
         </is>
       </c>
       <c r="C147" t="n">
-        <v>-0.00474229742353735</v>
+        <v>-0.004743678114212477</v>
       </c>
     </row>
     <row r="148">
@@ -2349,11 +2349,11 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>[-2, 6, -7]</t>
+          <t>[-7, 2, -1]</t>
         </is>
       </c>
       <c r="C148" t="n">
-        <v>-0.004743678114212477</v>
+        <v>-0.004490505448063682</v>
       </c>
     </row>
     <row r="149">
@@ -2362,11 +2362,11 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>[-7, 0, -2]</t>
+          <t>[-2, -2, -7]</t>
         </is>
       </c>
       <c r="C149" t="n">
-        <v>-0.004175700872249424</v>
+        <v>-0.003907652448724997</v>
       </c>
     </row>
     <row r="150">
@@ -2375,11 +2375,11 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>[-2, -2, -7]</t>
+          <t>[-2, 7, -3]</t>
         </is>
       </c>
       <c r="C150" t="n">
-        <v>-0.003907652448724997</v>
+        <v>-0.004743151701416048</v>
       </c>
     </row>
     <row r="151">
@@ -2388,11 +2388,11 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>[-2, 7, -3]</t>
+          <t>[2, 7, -3]</t>
         </is>
       </c>
       <c r="C151" t="n">
-        <v>-0.004743151701416048</v>
+        <v>-0.004744357296260861</v>
       </c>
     </row>
     <row r="152">
@@ -2401,11 +2401,11 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>[2, 7, -3]</t>
+          <t>[0, 0, -3]</t>
         </is>
       </c>
       <c r="C152" t="n">
-        <v>-0.004744357296260861</v>
+        <v>0.00182962296106711</v>
       </c>
     </row>
     <row r="153">
@@ -2414,11 +2414,11 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>[0, 0, -3]</t>
+          <t>[-6, -3, -7]</t>
         </is>
       </c>
       <c r="C153" t="n">
-        <v>0.00182962296106711</v>
+        <v>-0.004557199152885119</v>
       </c>
     </row>
     <row r="154">
@@ -2427,11 +2427,11 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>[-6, -3, -7]</t>
+          <t>[-4, -3, -7]</t>
         </is>
       </c>
       <c r="C154" t="n">
-        <v>-0.004557199152885119</v>
+        <v>-0.004481417157121379</v>
       </c>
     </row>
     <row r="155">
@@ -2440,11 +2440,11 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>[-4, -3, -7]</t>
+          <t>[-4, 0, -7]</t>
         </is>
       </c>
       <c r="C155" t="n">
-        <v>-0.004481417157121379</v>
+        <v>-0.002923372903447109</v>
       </c>
     </row>
     <row r="156">
@@ -2453,11 +2453,11 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>[-4, 0, -7]</t>
+          <t>[-7, 1, -4]</t>
         </is>
       </c>
       <c r="C156" t="n">
-        <v>-0.002923372903447109</v>
+        <v>-0.004339268392738302</v>
       </c>
     </row>
     <row r="157">
@@ -2466,11 +2466,11 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>[-7, 1, -4]</t>
+          <t>[-2, 4, -7]</t>
         </is>
       </c>
       <c r="C157" t="n">
-        <v>-0.004339268392738302</v>
+        <v>-0.004666224370621072</v>
       </c>
     </row>
     <row r="158">
@@ -2479,11 +2479,11 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>[-2, 4, -7]</t>
+          <t>[-7, -5, -1]</t>
         </is>
       </c>
       <c r="C158" t="n">
-        <v>-0.004666224370621072</v>
+        <v>-0.004715546041036716</v>
       </c>
     </row>
     <row r="159">
@@ -2492,11 +2492,11 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>[-7, -5, -1]</t>
+          <t>[1, 0, -7]</t>
         </is>
       </c>
       <c r="C159" t="n">
-        <v>-0.004715546041036716</v>
+        <v>-0.0009587502211900273</v>
       </c>
     </row>
     <row r="160">
@@ -2505,11 +2505,11 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>[1, 0, -7]</t>
+          <t>[-7, -3, -1]</t>
         </is>
       </c>
       <c r="C160" t="n">
-        <v>-0.0009587502211900273</v>
+        <v>-0.004575778317564122</v>
       </c>
     </row>
     <row r="161">
@@ -2518,11 +2518,11 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>[-7, -3, -1]</t>
+          <t>[-1, 7, 0]</t>
         </is>
       </c>
       <c r="C161" t="n">
-        <v>-0.004575778317564122</v>
+        <v>-0.004741898478231205</v>
       </c>
     </row>
     <row r="162">
@@ -2531,11 +2531,11 @@
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>[-1, 7, 0]</t>
+          <t>[-7, -3, 0]</t>
         </is>
       </c>
       <c r="C162" t="n">
-        <v>-0.004741898478231205</v>
+        <v>-0.004575683923589709</v>
       </c>
     </row>
     <row r="163">
@@ -2544,11 +2544,11 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>[-7, -3, 0]</t>
+          <t>[-6, 1, -7]</t>
         </is>
       </c>
       <c r="C163" t="n">
-        <v>-0.004575683923589709</v>
+        <v>-0.004242261327278391</v>
       </c>
     </row>
     <row r="164">
@@ -2557,11 +2557,11 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>[-6, 1, -7]</t>
+          <t>[-7, -6, -1]</t>
         </is>
       </c>
       <c r="C164" t="n">
-        <v>-0.004242261327278391</v>
+        <v>-0.004738183582922688</v>
       </c>
     </row>
     <row r="165">
@@ -2570,11 +2570,11 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>[-7, -6, -1]</t>
+          <t>[-7, 6, 4]</t>
         </is>
       </c>
       <c r="C165" t="n">
-        <v>-0.004738183582922688</v>
+        <v>-0.004742961488676329</v>
       </c>
     </row>
     <row r="166">
@@ -2583,11 +2583,11 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>[-7, 6, 4]</t>
+          <t>[-3, 2, -7]</t>
         </is>
       </c>
       <c r="C166" t="n">
-        <v>-0.004742961488676329</v>
+        <v>-0.004257764613417705</v>
       </c>
     </row>
     <row r="167">
@@ -2596,11 +2596,11 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>[-3, 2, -7]</t>
+          <t>[-7, 4, -4]</t>
         </is>
       </c>
       <c r="C167" t="n">
-        <v>-0.004257764613417705</v>
+        <v>-0.004692593645668491</v>
       </c>
     </row>
     <row r="168">
@@ -2609,11 +2609,11 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>[-7, 4, -4]</t>
+          <t>[-3, 6, -7]</t>
         </is>
       </c>
       <c r="C168" t="n">
-        <v>-0.004692593645668491</v>
+        <v>-0.004743730785828714</v>
       </c>
     </row>
     <row r="169">
@@ -2622,11 +2622,11 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>[-3, 6, -7]</t>
+          <t>[-2, 1, -1]</t>
         </is>
       </c>
       <c r="C169" t="n">
-        <v>-0.004743730785828714</v>
+        <v>-0.003096145677837171</v>
       </c>
     </row>
     <row r="170">
@@ -2635,11 +2635,11 @@
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>[-2, 1, -1]</t>
+          <t>[-1, 7, -3]</t>
         </is>
       </c>
       <c r="C170" t="n">
-        <v>-0.003096145677837171</v>
+        <v>-0.004743387763150972</v>
       </c>
     </row>
     <row r="171">
@@ -2648,11 +2648,11 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>[-1, 7, -3]</t>
+          <t>[0, 3, -3]</t>
         </is>
       </c>
       <c r="C171" t="n">
-        <v>-0.004743387763150972</v>
+        <v>-0.004528962883797141</v>
       </c>
     </row>
     <row r="172">
@@ -2661,11 +2661,11 @@
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>[0, 3, -3]</t>
+          <t>[-7, 2, -5]</t>
         </is>
       </c>
       <c r="C172" t="n">
-        <v>-0.004528962883797141</v>
+        <v>-0.004514763875044385</v>
       </c>
     </row>
     <row r="173">
@@ -2674,11 +2674,11 @@
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>[-7, 2, -5]</t>
+          <t>[-2, 2, -5]</t>
         </is>
       </c>
       <c r="C173" t="n">
-        <v>-0.004514763875044385</v>
+        <v>-0.004207672461566538</v>
       </c>
     </row>
     <row r="174">
@@ -2687,11 +2687,11 @@
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>[-2, 2, -5]</t>
+          <t>[-5, 5, -7]</t>
         </is>
       </c>
       <c r="C174" t="n">
-        <v>-0.004207672461566538</v>
+        <v>-0.004726304453181871</v>
       </c>
     </row>
     <row r="175">
@@ -2700,11 +2700,11 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>[0, 7, 0]</t>
+          <t>[-6, -5, -7]</t>
         </is>
       </c>
       <c r="C175" t="n">
-        <v>-0.004742343959420395</v>
+        <v>-0.004714238920067964</v>
       </c>
     </row>
     <row r="176">
@@ -2713,11 +2713,11 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>[-6, -5, -7]</t>
+          <t>[-1, -6, -7]</t>
         </is>
       </c>
       <c r="C176" t="n">
-        <v>-0.004714238920067964</v>
+        <v>-0.00473682005290208</v>
       </c>
     </row>
     <row r="177">
@@ -2726,11 +2726,11 @@
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>[-1, -6, -7]</t>
+          <t>[7, 3, -7]</t>
         </is>
       </c>
       <c r="C177" t="n">
-        <v>-0.00473682005290208</v>
+        <v>-0.004654392865634445</v>
       </c>
     </row>
     <row r="178">
@@ -2739,11 +2739,11 @@
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>[-7, 2, 2]</t>
+          <t>[0, -6, -7]</t>
         </is>
       </c>
       <c r="C178" t="n">
-        <v>-0.004493956305345495</v>
+        <v>-0.004736997867036617</v>
       </c>
     </row>
     <row r="179">
@@ -2752,11 +2752,11 @@
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>[0, -7, -7]</t>
+          <t>[-4, 2, -7]</t>
         </is>
       </c>
       <c r="C179" t="n">
-        <v>-0.004745695436888508</v>
+        <v>-0.004321283892867797</v>
       </c>
     </row>
     <row r="180">
@@ -2765,11 +2765,11 @@
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>[-3, -3, -7]</t>
+          <t>[0, -5, -7]</t>
         </is>
       </c>
       <c r="C180" t="n">
-        <v>-0.004453138648936791</v>
+        <v>-0.00470357573147531</v>
       </c>
     </row>
     <row r="181">
@@ -2778,11 +2778,11 @@
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>[0, -5, -7]</t>
+          <t>[0, -2, -7]</t>
         </is>
       </c>
       <c r="C181" t="n">
-        <v>-0.00470357573147531</v>
+        <v>-0.003885479472839625</v>
       </c>
     </row>
     <row r="182">
@@ -2791,11 +2791,11 @@
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>[6, 4, -7]</t>
+          <t>[-2, 0, -7]</t>
         </is>
       </c>
       <c r="C182" t="n">
-        <v>-0.004696594730820593</v>
+        <v>-8.271217424327126e-06</v>
       </c>
     </row>
     <row r="183">
@@ -2804,11 +2804,11 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>[-4, 2, -7]</t>
+          <t>[0, -1, -7]</t>
         </is>
       </c>
       <c r="C183" t="n">
-        <v>-0.004321283892843894</v>
+        <v>-0.001776055441700065</v>
       </c>
     </row>
     <row r="184">
@@ -2817,11 +2817,11 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>[0, -1, -7]</t>
+          <t>[5, 0, -7]</t>
         </is>
       </c>
       <c r="C184" t="n">
-        <v>-0.001776055441700065</v>
+        <v>-0.004071769240326352</v>
       </c>
     </row>
     <row r="185">
@@ -2830,11 +2830,11 @@
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>[-2, 0, -7]</t>
+          <t>[-3, 5, -7]</t>
         </is>
       </c>
       <c r="C185" t="n">
-        <v>-8.271222443242965e-06</v>
+        <v>-0.004723313393199368</v>
       </c>
     </row>
     <row r="186">
@@ -2843,11 +2843,11 @@
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>[-2, -7, -7]</t>
+          <t>[-7, -6, -5]</t>
         </is>
       </c>
       <c r="C186" t="n">
-        <v>-0.0047455788433707</v>
+        <v>-0.004739364717581528</v>
       </c>
     </row>
     <row r="187">
@@ -2856,11 +2856,11 @@
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>[0, -4, -7]</t>
+          <t>[0, -7, -7]</t>
         </is>
       </c>
       <c r="C187" t="n">
-        <v>-0.004623042396585984</v>
+        <v>-0.004745695436890326</v>
       </c>
     </row>
     <row r="188">
@@ -2869,11 +2869,11 @@
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>[-7, -3, -2]</t>
+          <t>[-7, -4, -1]</t>
         </is>
       </c>
       <c r="C188" t="n">
-        <v>-0.00457674028260936</v>
+        <v>-0.004666696841045672</v>
       </c>
     </row>
     <row r="189">
@@ -2882,11 +2882,11 @@
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>[-3, 5, -7]</t>
+          <t>[-7, 0, -5]</t>
         </is>
       </c>
       <c r="C189" t="n">
-        <v>-0.004723313393199368</v>
+        <v>-0.004240618754245893</v>
       </c>
     </row>
     <row r="190">
@@ -2895,11 +2895,11 @@
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>[-7, -6, -5]</t>
+          <t>[-3, -3, -7]</t>
         </is>
       </c>
       <c r="C190" t="n">
-        <v>-0.004739364717581528</v>
+        <v>-0.004453138648944644</v>
       </c>
     </row>
     <row r="191">
@@ -2908,11 +2908,11 @@
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>[-4, -2, -7]</t>
+          <t>[-7, 4, -2]</t>
         </is>
       </c>
       <c r="C191" t="n">
-        <v>-0.004122923060955744</v>
+        <v>-0.004689994084456059</v>
       </c>
     </row>
     <row r="192">
@@ -2921,11 +2921,11 @@
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>[-7, -4, -1]</t>
+          <t>[-3, 1, -7]</t>
         </is>
       </c>
       <c r="C192" t="n">
-        <v>-0.004666696841045672</v>
+        <v>-0.003454621176379012</v>
       </c>
     </row>
     <row r="193">
@@ -2934,11 +2934,11 @@
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>[-7, 0, -5]</t>
+          <t>[-3, -6, -7]</t>
         </is>
       </c>
       <c r="C193" t="n">
-        <v>-0.004240618754245893</v>
+        <v>-0.004736954253438608</v>
       </c>
     </row>
     <row r="194">
@@ -2947,11 +2947,11 @@
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>[-5, 5, -7]</t>
+          <t>[-7, 2, -4]</t>
         </is>
       </c>
       <c r="C194" t="n">
-        <v>-0.004726304453181153</v>
+        <v>-0.004505635847107952</v>
       </c>
     </row>
     <row r="195">
@@ -2960,11 +2960,11 @@
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>[-5, -2, -7]</t>
+          <t>[0, -4, -7]</t>
         </is>
       </c>
       <c r="C195" t="n">
-        <v>-0.00425325055489744</v>
+        <v>-0.004623042396570112</v>
       </c>
     </row>
     <row r="196">
@@ -2973,11 +2973,11 @@
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>[-6, 7, -2]</t>
+          <t>[-7, -2, -1]</t>
         </is>
       </c>
       <c r="C196" t="n">
-        <v>-0.004743188415628033</v>
+        <v>-0.004424015570255266</v>
       </c>
     </row>
     <row r="197">
@@ -2986,11 +2986,11 @@
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>[-4, -7, -7]</t>
+          <t>[-5, -1, -7]</t>
         </is>
       </c>
       <c r="C197" t="n">
-        <v>-0.004745528753045009</v>
+        <v>-0.003811393614758338</v>
       </c>
     </row>
     <row r="198">
@@ -2999,11 +2999,11 @@
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>[-3, 1, -7]</t>
+          <t>[-1, -2, -7]</t>
         </is>
       </c>
       <c r="C198" t="n">
-        <v>-0.003454621176379012</v>
+        <v>-0.003866326575092655</v>
       </c>
     </row>
     <row r="199">
@@ -3012,11 +3012,11 @@
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>[-1, -1, -7]</t>
+          <t>[4, 0, -7]</t>
         </is>
       </c>
       <c r="C199" t="n">
-        <v>-0.001589939407681792</v>
+        <v>-0.003742388299332865</v>
       </c>
     </row>
     <row r="200">
@@ -3025,11 +3025,11 @@
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>[7, 0, -7]</t>
+          <t>[-7, 2, -6]</t>
         </is>
       </c>
       <c r="C200" t="n">
-        <v>-0.00442842333046749</v>
+        <v>-0.004525034683963426</v>
       </c>
     </row>
     <row r="201">
@@ -3038,11 +3038,11 @@
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>[-7, -6, 0]</t>
+          <t>[-3, -5, -7]</t>
         </is>
       </c>
       <c r="C201" t="n">
-        <v>-0.004738139679801749</v>
+        <v>-0.00470470816184008</v>
       </c>
     </row>
     <row r="202">
@@ -3051,11 +3051,11 @@
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>[2, 0, -7]</t>
+          <t>[7, 0, -7]</t>
         </is>
       </c>
       <c r="C202" t="n">
-        <v>-0.00234676604636879</v>
+        <v>-0.00442842333046749</v>
       </c>
     </row>
     <row r="203">
@@ -3064,11 +3064,11 @@
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>[-6, 0, -1]</t>
+          <t>[-7, -6, 0]</t>
         </is>
       </c>
       <c r="C203" t="n">
-        <v>-0.003935110538050068</v>
+        <v>-0.004738139679801749</v>
       </c>
     </row>
     <row r="204">
@@ -3077,11 +3077,11 @@
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>[-7, 4, -1]</t>
+          <t>[2, 0, -7]</t>
         </is>
       </c>
       <c r="C204" t="n">
-        <v>-0.0046892889076463</v>
+        <v>-0.00234676604636879</v>
       </c>
     </row>
     <row r="205">
@@ -3090,11 +3090,11 @@
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>[1, 4, -7]</t>
+          <t>[-6, 0, -1]</t>
         </is>
       </c>
       <c r="C205" t="n">
-        <v>-0.004667027241331275</v>
+        <v>-0.003935110538050068</v>
       </c>
     </row>
     <row r="206">
@@ -3103,11 +3103,11 @@
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>[-1, -3, -7]</t>
+          <t>[-7, 4, -1]</t>
         </is>
       </c>
       <c r="C206" t="n">
-        <v>-0.004427182340501056</v>
+        <v>-0.0046892889076463</v>
       </c>
     </row>
     <row r="207">
@@ -3116,11 +3116,11 @@
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>[-3, 1, -2]</t>
+          <t>[1, 4, -7]</t>
         </is>
       </c>
       <c r="C207" t="n">
-        <v>-0.003459449700516605</v>
+        <v>-0.004667027241331275</v>
       </c>
     </row>
     <row r="208">
@@ -3129,11 +3129,11 @@
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>[-3, -7, -7]</t>
+          <t>[-1, -3, -7]</t>
         </is>
       </c>
       <c r="C208" t="n">
-        <v>-0.004745538054088319</v>
+        <v>-0.004427182340501056</v>
       </c>
     </row>
     <row r="209">
@@ -3142,11 +3142,11 @@
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>[-1, 7, -4]</t>
+          <t>[-2, 1, -3]</t>
         </is>
       </c>
       <c r="C209" t="n">
-        <v>-0.004743917384138884</v>
+        <v>-0.003131711541517939</v>
       </c>
     </row>
     <row r="210">
@@ -3155,11 +3155,11 @@
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>[5, 7, -4]</t>
+          <t>[-1, 1, -2]</t>
         </is>
       </c>
       <c r="C210" t="n">
-        <v>-0.004745182805996302</v>
+        <v>-0.002901261579900393</v>
       </c>
     </row>
     <row r="211">
@@ -3168,11 +3168,11 @@
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>[-1, -2, -7]</t>
+          <t>[-1, 7, -4]</t>
         </is>
       </c>
       <c r="C211" t="n">
-        <v>-0.003866326575367707</v>
+        <v>-0.004743917384138884</v>
       </c>
     </row>
     <row r="212">
@@ -3181,11 +3181,11 @@
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>[-6, -1, -7]</t>
+          <t>[5, 7, -4]</t>
         </is>
       </c>
       <c r="C212" t="n">
-        <v>-0.004130728838704696</v>
+        <v>-0.004745182805996302</v>
       </c>
     </row>
     <row r="213">
@@ -3194,11 +3194,11 @@
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>[0, -6, -7]</t>
+          <t>[-7, 0, 6]</t>
         </is>
       </c>
       <c r="C213" t="n">
-        <v>-0.004736997867035025</v>
+        <v>-0.004244770173784413</v>
       </c>
     </row>
     <row r="214">
@@ -3207,11 +3207,11 @@
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>[0, -3, -7]</t>
+          <t>[-2, -5, -7]</t>
         </is>
       </c>
       <c r="C214" t="n">
-        <v>-0.004431088660722334</v>
+        <v>-0.004703485937864108</v>
       </c>
     </row>
     <row r="215">
@@ -3220,11 +3220,11 @@
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>[-3, -6, -7]</t>
+          <t>[-1, -1, -7]</t>
         </is>
       </c>
       <c r="C215" t="n">
-        <v>-0.004736954253438518</v>
+        <v>-0.001589939409001509</v>
       </c>
     </row>
     <row r="216">
@@ -3233,11 +3233,11 @@
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>[-5, 1, -7]</t>
+          <t>[3, 1, -7]</t>
         </is>
       </c>
       <c r="C216" t="n">
-        <v>-0.004029266239617779</v>
+        <v>-0.003852208947514378</v>
       </c>
     </row>
     <row r="217">
@@ -3246,11 +3246,11 @@
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>[4, 2, -7]</t>
+          <t>[-7, -7, -3]</t>
         </is>
       </c>
       <c r="C217" t="n">
-        <v>-0.004407144037730484</v>
+        <v>-0.004744589604657373</v>
       </c>
     </row>
     <row r="218">
@@ -3259,11 +3259,11 @@
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>[0, 5, -7]</t>
+          <t>[6, 4, -7]</t>
         </is>
       </c>
       <c r="C218" t="n">
-        <v>-0.004722214032049807</v>
+        <v>-0.004696594730820479</v>
       </c>
     </row>
     <row r="219">
@@ -3272,11 +3272,11 @@
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>[0, -2, -7]</t>
+          <t>[0, -3, -7]</t>
         </is>
       </c>
       <c r="C219" t="n">
-        <v>-0.00388547947293264</v>
+        <v>-0.004431088660726421</v>
       </c>
     </row>
     <row r="220">
@@ -3285,11 +3285,11 @@
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>[-5, -1, -7]</t>
+          <t>[0, 5, -7]</t>
         </is>
       </c>
       <c r="C220" t="n">
-        <v>-0.003811393615087489</v>
+        <v>-0.004722214032049865</v>
       </c>
     </row>
     <row r="221">
@@ -3298,11 +3298,11 @@
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>[-7, -7, -5]</t>
+          <t>[-5, 1, -7]</t>
         </is>
       </c>
       <c r="C221" t="n">
-        <v>-0.004745316536139718</v>
+        <v>-0.004029266239617779</v>
       </c>
     </row>
     <row r="222">
@@ -3311,11 +3311,11 @@
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>[5, 1, -7]</t>
+          <t>[4, 2, -7]</t>
         </is>
       </c>
       <c r="C222" t="n">
-        <v>-0.004253536870203582</v>
+        <v>-0.004407144037730484</v>
       </c>
     </row>
     <row r="223">
@@ -3324,11 +3324,11 @@
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>[-7, 0, -6]</t>
+          <t>[-3, -4, -7]</t>
         </is>
       </c>
       <c r="C223" t="n">
-        <v>-0.004272145849863069</v>
+        <v>-0.004628403395598979</v>
       </c>
     </row>
     <row r="224">
@@ -3337,11 +3337,11 @@
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>[-2, -1, -7]</t>
+          <t>[-4, -4, -7]</t>
         </is>
       </c>
       <c r="C224" t="n">
-        <v>-0.002006725975469203</v>
+        <v>-0.004636262994682287</v>
       </c>
     </row>
     <row r="225">
@@ -3350,11 +3350,11 @@
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>[-1, 7, -6]</t>
+          <t>[2, 7, -7]</t>
         </is>
       </c>
       <c r="C225" t="n">
-        <v>-0.004744637371471993</v>
+        <v>-0.004745132344207956</v>
       </c>
     </row>
     <row r="226">
@@ -3363,11 +3363,11 @@
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>[-1, 5, -6]</t>
+          <t>[-7, -7, -5]</t>
         </is>
       </c>
       <c r="C226" t="n">
-        <v>-0.004721918780349316</v>
+        <v>-0.004745316536139718</v>
       </c>
     </row>
     <row r="227">
@@ -3376,11 +3376,11 @@
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>[1, 1, -7]</t>
+          <t>[-2, 0, -1]</t>
         </is>
       </c>
       <c r="C227" t="n">
-        <v>-0.003302320813929679</v>
+        <v>0.0006164037091191598</v>
       </c>
     </row>
     <row r="228">
@@ -3389,11 +3389,11 @@
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>[-5, -7, -7]</t>
+          <t>[-7, 0, -6]</t>
         </is>
       </c>
       <c r="C228" t="n">
-        <v>-0.004745576118086597</v>
+        <v>-0.004272145849863069</v>
       </c>
     </row>
     <row r="229">
@@ -3402,11 +3402,11 @@
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>[5, 0, -7]</t>
+          <t>[-2, -1, -7]</t>
         </is>
       </c>
       <c r="C229" t="n">
-        <v>-0.004071769240375996</v>
+        <v>-0.002006725975469203</v>
       </c>
     </row>
     <row r="230">
@@ -3415,11 +3415,11 @@
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>[4, 0, -7]</t>
+          <t>[-1, 7, -6]</t>
         </is>
       </c>
       <c r="C230" t="n">
-        <v>-0.003742388299374708</v>
+        <v>-0.004744637371471993</v>
       </c>
     </row>
     <row r="231">
@@ -3428,11 +3428,11 @@
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>[-3, -5, -7]</t>
+          <t>[-1, 5, -6]</t>
         </is>
       </c>
       <c r="C231" t="n">
-        <v>-0.004704708161838871</v>
+        <v>-0.004721918780349316</v>
       </c>
     </row>
     <row r="232">
@@ -3441,11 +3441,11 @@
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>[0, 2, 0]</t>
+          <t>[-2, -7, -7]</t>
         </is>
       </c>
       <c r="C232" t="n">
-        <v>-0.004170408981564087</v>
+        <v>-0.004745578843369158</v>
       </c>
     </row>
     <row r="233">
@@ -3454,11 +3454,11 @@
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>[3, 7, -7]</t>
+          <t>[-6, 3, -7]</t>
         </is>
       </c>
       <c r="C233" t="n">
-        <v>-0.004745240721231841</v>
+        <v>-0.004610440003359261</v>
       </c>
     </row>
     <row r="234">
@@ -3467,11 +3467,11 @@
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>[3, 1, -7]</t>
+          <t>[1, 5, -7]</t>
         </is>
       </c>
       <c r="C234" t="n">
-        <v>-0.003852208947481395</v>
+        <v>-0.004722691325162538</v>
       </c>
     </row>
     <row r="235">
@@ -3480,11 +3480,11 @@
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>[-6, 5, -7]</t>
+          <t>[1, 1, -7]</t>
         </is>
       </c>
       <c r="C235" t="n">
-        <v>-0.004728491676504453</v>
+        <v>-0.003302320813929679</v>
       </c>
     </row>
     <row r="236">
@@ -3493,11 +3493,11 @@
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>[6, 1, -7]</t>
+          <t>[-5, -7, -7]</t>
         </is>
       </c>
       <c r="C236" t="n">
-        <v>-0.004387244697583835</v>
+        <v>-0.004745576118086597</v>
       </c>
     </row>
     <row r="237">
@@ -3506,11 +3506,11 @@
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>[-1, 1, -3]</t>
+          <t>[-1, 0, -1]</t>
         </is>
       </c>
       <c r="C237" t="n">
-        <v>-0.002934157688238304</v>
+        <v>0.00366203389383782</v>
       </c>
     </row>
     <row r="238">
@@ -3519,11 +3519,11 @@
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>[-1, 0, -1]</t>
+          <t>[4, 1, -7]</t>
         </is>
       </c>
       <c r="C238" t="n">
-        <v>0.003662033905396223</v>
+        <v>-0.004077367377234332</v>
       </c>
     </row>
     <row r="239">
@@ -3532,11 +3532,11 @@
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>[4, 6, -7]</t>
+          <t>[5, 1, -7]</t>
         </is>
       </c>
       <c r="C239" t="n">
-        <v>-0.004744247206544896</v>
+        <v>-0.004253536870285878</v>
       </c>
     </row>
     <row r="240">
@@ -3545,11 +3545,11 @@
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>[0, 7, -2]</t>
+          <t>[-7, 0, -2]</t>
         </is>
       </c>
       <c r="C240" t="n">
-        <v>-0.004743178694826868</v>
+        <v>-0.004175700872288238</v>
       </c>
     </row>
     <row r="241">
@@ -3558,11 +3558,11 @@
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>[0, 4, -2]</t>
+          <t>[-3, 0, -2]</t>
         </is>
       </c>
       <c r="C241" t="n">
-        <v>-0.004662249092657019</v>
+        <v>-0.001823363151101517</v>
       </c>
     </row>
     <row r="242">
@@ -3571,11 +3571,11 @@
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>[5, 2, -7]</t>
+          <t>[-3, 7, -2]</t>
         </is>
       </c>
       <c r="C242" t="n">
-        <v>-0.004470513854416556</v>
+        <v>-0.004742460829349655</v>
       </c>
     </row>
     <row r="243">
@@ -3584,11 +3584,11 @@
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>[-2, -5, -7]</t>
+          <t>[1, 7, -3]</t>
         </is>
       </c>
       <c r="C243" t="n">
-        <v>-0.004703485937864194</v>
+        <v>-0.0047440418905544</v>
       </c>
     </row>
     <row r="244">
@@ -3597,11 +3597,11 @@
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>[-1, 0, -3]</t>
+          <t>[3, 7, -7]</t>
         </is>
       </c>
       <c r="C244" t="n">
-        <v>0.002724768243854251</v>
+        <v>-0.004745240721231841</v>
       </c>
     </row>
     <row r="245">
@@ -3610,11 +3610,11 @@
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>[-4, -4, -7]</t>
+          <t>[-1, 0, -2]</t>
         </is>
       </c>
       <c r="C245" t="n">
-        <v>-0.004636262994683367</v>
+        <v>0.003209784709427488</v>
       </c>
     </row>
     <row r="246">
@@ -3623,11 +3623,11 @@
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>[-2, 0, -1]</t>
+          <t>[-6, 5, -7]</t>
         </is>
       </c>
       <c r="C246" t="n">
-        <v>0.0006164037122631271</v>
+        <v>-0.004728491676504453</v>
       </c>
     </row>
     <row r="247">
@@ -3636,11 +3636,11 @@
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>[2, 7, -7]</t>
+          <t>[6, 1, -7]</t>
         </is>
       </c>
       <c r="C247" t="n">
-        <v>-0.004745132344207841</v>
+        <v>-0.004387244697583835</v>
       </c>
     </row>
     <row r="248">
@@ -3649,11 +3649,11 @@
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>[3, 4, -7]</t>
+          <t>[-1, 1, -3]</t>
         </is>
       </c>
       <c r="C248" t="n">
-        <v>-0.004675455918009911</v>
+        <v>-0.002934157688238304</v>
       </c>
     </row>
     <row r="249">
@@ -3662,11 +3662,11 @@
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>[-1, 0, -2]</t>
+          <t>[0, 0, -2]</t>
         </is>
       </c>
       <c r="C249" t="n">
-        <v>0.003209784719156836</v>
+        <v>0.002285723648222364</v>
       </c>
     </row>
     <row r="250">
@@ -3675,11 +3675,11 @@
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>[0, 0, 0]</t>
+          <t>[5, 2, -7]</t>
         </is>
       </c>
       <c r="C250" t="n">
-        <v>0.003153329476870075</v>
+        <v>-0.004470513854416556</v>
       </c>
     </row>
     <row r="251">
@@ -3688,11 +3688,11 @@
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>[0, 0, -6]</t>
+          <t>[-5, 7, -1]</t>
         </is>
       </c>
       <c r="C251" t="n">
-        <v>0.000928379179733565</v>
+        <v>-0.004742537387391745</v>
       </c>
     </row>
     <row r="252">
@@ -3701,11 +3701,11 @@
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>[7, 4, -7]</t>
+          <t>[-1, 0, -3]</t>
         </is>
       </c>
       <c r="C252" t="n">
-        <v>-0.004704701885593208</v>
+        <v>0.002724768243854251</v>
       </c>
     </row>
     <row r="253">
@@ -3714,11 +3714,11 @@
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>[6, 6, -7]</t>
+          <t>[-1, 0, -4]</t>
         </is>
       </c>
       <c r="C253" t="n">
-        <v>-0.004744771343335659</v>
+        <v>0.002272245532972156</v>
       </c>
     </row>
     <row r="254">
@@ -3727,11 +3727,11 @@
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>[-1, 0, 0]</t>
+          <t>[0, 0, 0]</t>
         </is>
       </c>
       <c r="C254" t="n">
-        <v>0.004011011772371727</v>
+        <v>0.003153329482738177</v>
       </c>
     </row>
     <row r="255">
@@ -3740,11 +3740,11 @@
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>[4, 4, -7]</t>
+          <t>[-1, 0, 0]</t>
         </is>
       </c>
       <c r="C255" t="n">
-        <v>-0.004681620930025426</v>
+        <v>0.004011011765132058</v>
       </c>
     </row>
     <row r="256">
@@ -3753,11 +3753,11 @@
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>[-1, 2, 0]</t>
+          <t>[3, 4, -7]</t>
         </is>
       </c>
       <c r="C256" t="n">
-        <v>-0.004162770259107712</v>
+        <v>-0.004675455918009911</v>
       </c>
     </row>
     <row r="257">
@@ -3766,11 +3766,11 @@
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>[5, 5, -7]</t>
+          <t>[-1, 5, 0]</t>
         </is>
       </c>
       <c r="C257" t="n">
-        <v>-0.00472841096147362</v>
+        <v>-0.004718839935166287</v>
       </c>
     </row>
     <row r="258">
@@ -3779,11 +3779,11 @@
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>[4, 3, -7]</t>
+          <t>[-3, 0, -1]</t>
         </is>
       </c>
       <c r="C258" t="n">
-        <v>-0.004589260504398992</v>
+        <v>-0.001725626455208825</v>
       </c>
     </row>
     <row r="259">
@@ -3792,11 +3792,11 @@
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>[0, 2, -1]</t>
+          <t>[-1, 3, -1]</t>
         </is>
       </c>
       <c r="C259" t="n">
-        <v>-0.004174032450156752</v>
+        <v>-0.004523785694072061</v>
       </c>
     </row>
     <row r="260">
@@ -3805,11 +3805,11 @@
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>[-1, 4, -6]</t>
+          <t>[-1, 0, -6]</t>
         </is>
       </c>
       <c r="C260" t="n">
-        <v>-0.004664444751600903</v>
+        <v>0.001601022747306309</v>
       </c>
     </row>
     <row r="261">
@@ -3818,11 +3818,11 @@
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>[-1, 0, -4]</t>
+          <t>[6, 6, -7]</t>
         </is>
       </c>
       <c r="C261" t="n">
-        <v>0.002272245580739185</v>
+        <v>-0.004744771343335659</v>
       </c>
     </row>
     <row r="262">
@@ -3831,11 +3831,11 @@
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>[-5, 7, -1]</t>
+          <t>[0, 0, -1]</t>
         </is>
       </c>
       <c r="C262" t="n">
-        <v>-0.004742537387391181</v>
+        <v>0.002741494954585536</v>
       </c>
     </row>
     <row r="263">
@@ -3844,11 +3844,11 @@
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>[0, 0, -1]</t>
+          <t>[0, 7, -6]</t>
         </is>
       </c>
       <c r="C263" t="n">
-        <v>0.002741494998601239</v>
+        <v>-0.004744750986299574</v>
       </c>
     </row>
     <row r="264">
@@ -3857,11 +3857,11 @@
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>[-1, 0, -5]</t>
+          <t>[0, 4, -6]</t>
         </is>
       </c>
       <c r="C264" t="n">
-        <v>0.001897098146199518</v>
+        <v>-0.004664770447305489</v>
       </c>
     </row>
     <row r="265">
@@ -3870,11 +3870,11 @@
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>[-3, 0, -3]</t>
+          <t>[-3, -7, -7]</t>
         </is>
       </c>
       <c r="C265" t="n">
-        <v>-0.001895270797042564</v>
+        <v>-0.004745538054088914</v>
       </c>
     </row>
     <row r="266">
@@ -3883,11 +3883,11 @@
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>[-1, 0, -6]</t>
+          <t>[-4, 0, -1]</t>
         </is>
       </c>
       <c r="C266" t="n">
-        <v>0.001601022746000906</v>
+        <v>-0.002927432264227617</v>
       </c>
     </row>
     <row r="267">
@@ -3896,11 +3896,11 @@
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>[0, 0, -2]</t>
+          <t>[-1, 4, -1]</t>
         </is>
       </c>
       <c r="C267" t="n">
-        <v>0.002285723640994261</v>
+        <v>-0.004660686072437599</v>
       </c>
     </row>
     <row r="268">
@@ -3909,11 +3909,11 @@
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>[-5, 3, -7]</t>
+          <t>[-1, 4, -6]</t>
         </is>
       </c>
       <c r="C268" t="n">
-        <v>-0.004585947615811971</v>
+        <v>-0.004664444751600903</v>
       </c>
     </row>
     <row r="269">
@@ -3922,11 +3922,11 @@
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>[1, 3, -7]</t>
+          <t>[-1, 0, -5]</t>
         </is>
       </c>
       <c r="C269" t="n">
-        <v>-0.004540276836460574</v>
+        <v>0.001897098146199518</v>
       </c>
     </row>
     <row r="270">
@@ -3935,11 +3935,11 @@
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>[-2, -4, -7]</t>
+          <t>[-3, 0, -3]</t>
         </is>
       </c>
       <c r="C270" t="n">
-        <v>-0.004623602277347025</v>
+        <v>-0.001895270797042564</v>
       </c>
     </row>
     <row r="271">
@@ -3948,11 +3948,11 @@
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>[0, 7, -5]</t>
+          <t>[4, 3, -7]</t>
         </is>
       </c>
       <c r="C271" t="n">
-        <v>-0.004744501656546535</v>
+        <v>-0.004589260504392057</v>
       </c>
     </row>
     <row r="272">
@@ -3961,11 +3961,11 @@
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>[-4, 0, -1]</t>
+          <t>[-1, 2, 0]</t>
         </is>
       </c>
       <c r="C272" t="n">
-        <v>-0.002927432264715443</v>
+        <v>-0.004162770259769482</v>
       </c>
     </row>
     <row r="273">
@@ -3974,11 +3974,11 @@
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>[-5, 0, -5]</t>
+          <t>[0, 0, -4]</t>
         </is>
       </c>
       <c r="C273" t="n">
-        <v>-0.003719268937656934</v>
+        <v>0.001447062165979395</v>
       </c>
     </row>
     <row r="274">
@@ -3987,11 +3987,11 @@
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>[-3, 0, -1]</t>
+          <t>[-4, 7, -2]</t>
         </is>
       </c>
       <c r="C274" t="n">
-        <v>-0.001725626454380056</v>
+        <v>-0.004742557812610877</v>
       </c>
     </row>
     <row r="275">
@@ -4000,11 +4000,11 @@
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>[-1, 4, 0]</t>
+          <t>[-5, 0, -5]</t>
         </is>
       </c>
       <c r="C275" t="n">
-        <v>-0.004660037287231514</v>
+        <v>-0.003719268937656934</v>
       </c>
     </row>
     <row r="276">
@@ -4013,11 +4013,11 @@
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>[2, 3, -7]</t>
+          <t>[0, 0, -6]</t>
         </is>
       </c>
       <c r="C276" t="n">
-        <v>-0.004552728258776156</v>
+        <v>0.0009283791846957701</v>
       </c>
     </row>
     <row r="277">
@@ -4026,11 +4026,11 @@
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>[2, 2, -7]</t>
+          <t>[-1, 4, 0]</t>
         </is>
       </c>
       <c r="C277" t="n">
-        <v>-0.004280031924036517</v>
+        <v>-0.004660037287231514</v>
       </c>
     </row>
     <row r="278">
@@ -4039,11 +4039,11 @@
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>[-2, 0, -3]</t>
+          <t>[2, 7, 0]</t>
         </is>
       </c>
       <c r="C278" t="n">
-        <v>0.0003830968239188715</v>
+        <v>-0.004743350161314597</v>
       </c>
     </row>
     <row r="279">
@@ -4052,11 +4052,11 @@
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>[-1, 4, -1]</t>
+          <t>[3, 2, -7]</t>
         </is>
       </c>
       <c r="C279" t="n">
-        <v>-0.004660686072451521</v>
+        <v>-0.00434175686232928</v>
       </c>
     </row>
     <row r="280">
@@ -4065,11 +4065,11 @@
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>[0, 0, -4]</t>
+          <t>[2, 7, -1]</t>
         </is>
       </c>
       <c r="C280" t="n">
-        <v>0.001447062166038862</v>
+        <v>-0.004743647437811547</v>
       </c>
     </row>
     <row r="281">
@@ -4078,11 +4078,11 @@
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>[-1, 3, 0]</t>
+          <t>[0, 0, -5]</t>
         </is>
       </c>
       <c r="C281" t="n">
-        <v>-0.004522502619890918</v>
+        <v>0.001151031935617537</v>
       </c>
     </row>
     <row r="282">
@@ -4091,11 +4091,11 @@
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>[0, 1, -1]</t>
+          <t>[-1, 1, 0]</t>
         </is>
       </c>
       <c r="C282" t="n">
-        <v>-0.002927450250511219</v>
+        <v>-0.002849322189403157</v>
       </c>
     </row>
     <row r="283">
@@ -4104,11 +4104,11 @@
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>[0, 0, -5]</t>
+          <t>[-2, 0, -5]</t>
         </is>
       </c>
       <c r="C283" t="n">
-        <v>0.001151031935617537</v>
+        <v>0.0002142749209860129</v>
       </c>
     </row>
     <row r="284">
@@ -4117,11 +4117,11 @@
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>[-1, 1, 0]</t>
+          <t>[-1, 2, -6]</t>
         </is>
       </c>
       <c r="C284" t="n">
-        <v>-0.002849322189403157</v>
+        <v>-0.004188662575366727</v>
       </c>
     </row>
     <row r="285">
@@ -4130,11 +4130,11 @@
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>[-2, 0, -5]</t>
+          <t>[-1, 2, -4]</t>
         </is>
       </c>
       <c r="C285" t="n">
-        <v>0.0002142749209860129</v>
+        <v>-0.004181277696554864</v>
       </c>
     </row>
     <row r="286">
@@ -4143,11 +4143,11 @@
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>[-1, 1, -2]</t>
+          <t>[1, 3, -7]</t>
         </is>
       </c>
       <c r="C286" t="n">
-        <v>-0.002901261575030826</v>
+        <v>-0.004540276836460559</v>
       </c>
     </row>
     <row r="287">
@@ -4156,11 +4156,11 @@
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>[-1, 2, -4]</t>
+          <t>[-2, 0, -6]</t>
         </is>
       </c>
       <c r="C287" t="n">
-        <v>-0.004181277696554864</v>
+        <v>0.0001035898042768868</v>
       </c>
     </row>
     <row r="288">
@@ -4169,11 +4169,11 @@
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>[-3, 0, -4]</t>
+          <t>[-1, 1, -6]</t>
         </is>
       </c>
       <c r="C288" t="n">
-        <v>-0.001853426884812612</v>
+        <v>-0.003017230295044536</v>
       </c>
     </row>
     <row r="289">
@@ -4182,11 +4182,11 @@
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>[-1, 1, -4]</t>
+          <t>[-1, 2, -2]</t>
         </is>
       </c>
       <c r="C289" t="n">
-        <v>-0.002966478619380471</v>
+        <v>-0.004171254865158522</v>
       </c>
     </row>
     <row r="290">
@@ -4195,11 +4195,11 @@
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>[-1, 1, -6]</t>
+          <t>[2, 2, -7]</t>
         </is>
       </c>
       <c r="C290" t="n">
-        <v>-0.003017230295044536</v>
+        <v>-0.004280031923994777</v>
       </c>
     </row>
     <row r="291">
@@ -4208,11 +4208,11 @@
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>[-1, 2, -2]</t>
+          <t>[-1, 3, -2]</t>
         </is>
       </c>
       <c r="C291" t="n">
-        <v>-0.004171254865158522</v>
+        <v>-0.004525361994120444</v>
       </c>
     </row>
     <row r="292">
@@ -4221,11 +4221,11 @@
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>[2, 7, 0]</t>
+          <t>[-1, 3, 0]</t>
         </is>
       </c>
       <c r="C292" t="n">
-        <v>-0.004743350161314425</v>
+        <v>-0.004522502619888184</v>
       </c>
     </row>
     <row r="293">
@@ -4234,11 +4234,11 @@
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>[-2, 0, 0]</t>
+          <t>[-1, 1, -4]</t>
         </is>
       </c>
       <c r="C293" t="n">
-        <v>0.0007280521370604143</v>
+        <v>-0.002966478619574614</v>
       </c>
     </row>
     <row r="294">
@@ -4247,11 +4247,11 @@
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>[-6, 7, -1]</t>
+          <t>[-2, 0, 0]</t>
         </is>
       </c>
       <c r="C294" t="n">
-        <v>-0.004742979510296451</v>
+        <v>0.0007280521370604143</v>
       </c>
     </row>
     <row r="295">
@@ -4260,24 +4260,11 @@
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>[-3, 0, 0]</t>
+          <t>[-4, 0, 0]</t>
         </is>
       </c>
       <c r="C295" t="n">
-        <v>-0.001667607106277731</v>
-      </c>
-    </row>
-    <row r="296">
-      <c r="A296" s="1" t="n">
-        <v>294</v>
-      </c>
-      <c r="B296" t="inlineStr">
-        <is>
-          <t>[-4, 0, 0]</t>
-        </is>
-      </c>
-      <c r="C296" t="n">
-        <v>-0.002892801373737466</v>
+        <v>-0.002892801374086874</v>
       </c>
     </row>
   </sheetData>

</xml_diff>